<commit_message>
finish first pass on curve fitting and visualize preliminary results. anecdotally looks like there's nothing there
</commit_message>
<xml_diff>
--- a/log/TT_tag_metadata.xlsx
+++ b/log/TT_tag_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eaperkowski/git/trillium_trail/log/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A2A5C2-78B1-7E44-9831-B4B440565B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B29DDC-712D-524C-B6D1-C22E6E1D1E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="500" windowWidth="44120" windowHeight="28220" xr2:uid="{C05A6612-8A40-464F-B145-5025FDD9DACD}"/>
+    <workbookView xWindow="51700" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{C05A6612-8A40-464F-B145-5025FDD9DACD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="12">
   <si>
     <t>plot</t>
   </si>
@@ -424,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B4D0198-D542-5A4D-94CB-070E79E04F7A}">
-  <dimension ref="A1:E146"/>
+  <dimension ref="A1:E147"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="370" zoomScaleNormal="370" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A139" zoomScale="370" zoomScaleNormal="370" workbookViewId="0">
+      <selection activeCell="B148" sqref="B148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2917,6 +2917,23 @@
         <v>11</v>
       </c>
     </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>5073</v>
+      </c>
+      <c r="B147" t="s">
+        <v>7</v>
+      </c>
+      <c r="C147">
+        <v>5</v>
+      </c>
+      <c r="D147">
+        <v>36</v>
+      </c>
+      <c r="E147" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E146">
     <sortCondition ref="C2:C146"/>

</xml_diff>